<commit_message>
Sort funktioniert + Fächer sind zu den Tutoren gespeichert
</commit_message>
<xml_diff>
--- a/01_Planning/ProductBacklog/ProductBacklog.xlsx
+++ b/01_Planning/ProductBacklog/ProductBacklog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t xml:space="preserve">#id </t>
   </si>
@@ -127,6 +127,12 @@
   </si>
   <si>
     <t>User can use website on mobile device</t>
+  </si>
+  <si>
+    <t>&lt;SP13&gt;</t>
+  </si>
+  <si>
+    <t>Teacher can log in</t>
   </si>
 </sst>
 </file>
@@ -529,7 +535,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -760,9 +766,20 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="11">
+        <v>2</v>
+      </c>
       <c r="E14" s="10">
-        <f>AVERAGE(E2:E13)</f>
-        <v>3.3333333333333335</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Tutor werden fast fertig (Bild fehlt, pro Account ein Tutor)
</commit_message>
<xml_diff>
--- a/01_Planning/ProductBacklog/ProductBacklog.xlsx
+++ b/01_Planning/ProductBacklog/ProductBacklog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="43">
   <si>
     <t xml:space="preserve">#id </t>
   </si>
@@ -87,9 +87,6 @@
     <t xml:space="preserve">&lt;SP9&gt; </t>
   </si>
   <si>
-    <t>User wants to review hist tutor</t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;SP4&gt; </t>
   </si>
   <si>
@@ -142,6 +139,15 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>User wants to review his tutor</t>
+  </si>
+  <si>
+    <t>Logic</t>
+  </si>
+  <si>
+    <t>Tested</t>
   </si>
 </sst>
 </file>
@@ -541,7 +547,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
@@ -553,7 +559,7 @@
     <col min="3" max="3" width="62" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -570,10 +576,19 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -590,10 +605,19 @@
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="G2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -612,8 +636,17 @@
       <c r="F3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
@@ -630,10 +663,19 @@
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="G4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
@@ -652,8 +694,17 @@
       <c r="F5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>17</v>
       </c>
@@ -670,10 +721,19 @@
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="G6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>19</v>
       </c>
@@ -692,8 +752,17 @@
       <c r="F7" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>21</v>
       </c>
@@ -701,7 +770,7 @@
         <v>15</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="D8" s="4">
         <v>2</v>
@@ -710,18 +779,27 @@
         <v>3</v>
       </c>
       <c r="F8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="G8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D9" s="4">
         <v>3</v>
@@ -730,18 +808,27 @@
         <v>3</v>
       </c>
       <c r="F9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="G9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" s="4">
         <v>3</v>
@@ -752,16 +839,25 @@
       <c r="F10" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G10" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" t="s">
+        <v>38</v>
+      </c>
+      <c r="I10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="D11" s="4">
         <v>3</v>
@@ -770,18 +866,27 @@
         <v>8</v>
       </c>
       <c r="F11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="G11" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="D12" s="4">
         <v>3</v>
@@ -790,18 +895,27 @@
         <v>3</v>
       </c>
       <c r="F12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="G12" t="s">
+        <v>39</v>
+      </c>
+      <c r="H12" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="C13" s="8" t="s">
         <v>34</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>35</v>
       </c>
       <c r="D13" s="11">
         <v>2</v>
@@ -812,16 +926,25 @@
       <c r="F13" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>36</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>37</v>
       </c>
       <c r="D14" s="11">
         <v>2</v>
@@ -830,16 +953,25 @@
         <v>3</v>
       </c>
       <c r="F14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="G14" t="s">
+        <v>39</v>
+      </c>
+      <c r="H14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="11"/>
     </row>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>

</xml_diff>

<commit_message>
filldb test with new telephone numbers
</commit_message>
<xml_diff>
--- a/01_Planning/ProductBacklog/ProductBacklog.xlsx
+++ b/01_Planning/ProductBacklog/ProductBacklog.xlsx
@@ -211,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -220,19 +220,16 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -550,7 +547,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -804,7 +801,7 @@
       <c r="D9" s="4">
         <v>3</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="11">
         <v>3</v>
       </c>
       <c r="F9" t="s">
@@ -850,7 +847,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -879,7 +876,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -891,7 +888,7 @@
       <c r="D12" s="4">
         <v>3</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="8">
         <v>3</v>
       </c>
       <c r="F12" t="s">
@@ -908,19 +905,19 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="11">
-        <v>2</v>
-      </c>
-      <c r="E13" s="9">
+      <c r="D13" s="9">
+        <v>2</v>
+      </c>
+      <c r="E13" s="8">
         <v>5</v>
       </c>
       <c r="F13" t="s">
@@ -937,19 +934,19 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="11">
-        <v>2</v>
-      </c>
-      <c r="E14" s="10">
+      <c r="D14" s="9">
+        <v>2</v>
+      </c>
+      <c r="E14" s="11">
         <v>3</v>
       </c>
       <c r="F14" t="s">
@@ -966,17 +963,17 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="7"/>
+      <c r="A15" s="6"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="11"/>
+      <c r="D15" s="9"/>
     </row>
     <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
-      <c r="E16" s="12"/>
+      <c r="E16" s="10"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5"/>

</xml_diff>

<commit_message>
Role Refreshing Bugs fixed
</commit_message>
<xml_diff>
--- a/01_Planning/ProductBacklog/ProductBacklog.xlsx
+++ b/01_Planning/ProductBacklog/ProductBacklog.xlsx
@@ -199,7 +199,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -222,6 +222,11 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -284,7 +289,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -302,6 +307,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
@@ -620,7 +626,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -732,8 +738,8 @@
       <c r="E4" s="6">
         <v>2</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>38</v>
+      <c r="F4" s="13" t="s">
+        <v>39</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>38</v>
@@ -1182,5 +1188,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
keck added as an admin
</commit_message>
<xml_diff>
--- a/01_Planning/ProductBacklog/ProductBacklog.xlsx
+++ b/01_Planning/ProductBacklog/ProductBacklog.xlsx
@@ -289,7 +289,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -306,7 +306,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -626,7 +625,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -738,11 +737,11 @@
       <c r="E4" s="6">
         <v>2</v>
       </c>
-      <c r="F4" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>38</v>
+      <c r="F4" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>38</v>
@@ -1118,8 +1117,8 @@
       <c r="F17" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="G17" s="5" t="s">
-        <v>38</v>
+      <c r="G17" s="11" t="s">
+        <v>39</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>38</v>
@@ -1147,8 +1146,8 @@
       <c r="F18" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="12" t="s">
-        <v>38</v>
+      <c r="G18" s="11" t="s">
+        <v>39</v>
       </c>
       <c r="H18" s="5" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
Planning up to date
</commit_message>
<xml_diff>
--- a/01_Planning/ProductBacklog/ProductBacklog.xlsx
+++ b/01_Planning/ProductBacklog/ProductBacklog.xlsx
@@ -625,7 +625,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="H15" sqref="H15:I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -743,11 +743,11 @@
       <c r="G4" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>38</v>
+      <c r="H4" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -801,11 +801,11 @@
       <c r="G6" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>38</v>
+      <c r="H6" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1062,11 +1062,11 @@
       <c r="G15" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="H15" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>38</v>
+      <c r="H15" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1091,11 +1091,11 @@
       <c r="G16" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="H16" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>38</v>
+      <c r="H16" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1120,11 +1120,11 @@
       <c r="G17" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="H17" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>38</v>
+      <c r="H17" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1149,11 +1149,11 @@
       <c r="G18" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="H18" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>38</v>
+      <c r="H18" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Send tutoring request code
</commit_message>
<xml_diff>
--- a/01_Planning/ProductBacklog/ProductBacklog.xlsx
+++ b/01_Planning/ProductBacklog/ProductBacklog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="63">
   <si>
     <t xml:space="preserve">#id </t>
   </si>
@@ -190,6 +190,24 @@
   </si>
   <si>
     <t>Tutors can add an image to their profile</t>
+  </si>
+  <si>
+    <t>&lt;SP19&gt;</t>
+  </si>
+  <si>
+    <t>&lt;SP20&gt;</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Teacher can filter tutors by subject in comment tutor page</t>
+  </si>
+  <si>
+    <t>Emails for admin</t>
+  </si>
+  <si>
+    <t>Admin can send E-Mails to an outstanding tutor</t>
   </si>
 </sst>
 </file>
@@ -289,7 +307,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -307,6 +325,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
@@ -622,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15:I18"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1098,7 +1117,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>48</v>
       </c>
@@ -1127,7 +1146,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>51</v>
       </c>
@@ -1156,7 +1175,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>54</v>
       </c>
@@ -1182,6 +1201,72 @@
         <v>38</v>
       </c>
       <c r="I19" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" s="5">
+        <v>2</v>
+      </c>
+      <c r="E20" s="5">
+        <v>1</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="13"/>
+    </row>
+    <row r="21" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" s="5">
+        <v>2</v>
+      </c>
+      <c r="E21" s="5">
+        <v>3</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I21" s="5" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
edit tutor bug fix
</commit_message>
<xml_diff>
--- a/01_Planning/ProductBacklog/ProductBacklog.xlsx
+++ b/01_Planning/ProductBacklog/ProductBacklog.xlsx
@@ -644,7 +644,7 @@
   <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -962,14 +962,14 @@
       <c r="F11" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="G11" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>38</v>
+      <c r="G11" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1194,14 +1194,14 @@
       <c r="F19" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="G19" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>38</v>
+      <c r="G19" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1223,14 +1223,14 @@
       <c r="F20" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="G20" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>38</v>
+      <c r="G20" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>39</v>
       </c>
       <c r="J20" s="13"/>
       <c r="K20" s="13"/>
@@ -1260,14 +1260,14 @@
       <c r="F21" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="G21" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>38</v>
+      <c r="G21" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edit Tutor accept/decline final bug fix
</commit_message>
<xml_diff>
--- a/01_Planning/ProductBacklog/ProductBacklog.xlsx
+++ b/01_Planning/ProductBacklog/ProductBacklog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="66">
   <si>
     <t xml:space="preserve">#id </t>
   </si>
@@ -208,6 +208,15 @@
   </si>
   <si>
     <t>Admin can send E-Mails to an outstanding tutor</t>
+  </si>
+  <si>
+    <t>Admin can see statistics</t>
+  </si>
+  <si>
+    <t>Tutor will get email when he/she is accepted</t>
+  </si>
+  <si>
+    <t>Admin can send mail to all tutors</t>
   </si>
 </sst>
 </file>
@@ -307,7 +316,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -326,6 +335,8 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
@@ -641,10 +652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q21"/>
+  <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1270,6 +1281,75 @@
         <v>39</v>
       </c>
     </row>
+    <row r="22" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C22" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" s="14">
+        <v>1</v>
+      </c>
+      <c r="E22" s="14">
+        <v>5</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="H22" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I22" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C23" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="14">
+        <v>2</v>
+      </c>
+      <c r="E23" s="14">
+        <v>2</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="H23" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I23" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C24" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" s="14">
+        <v>2</v>
+      </c>
+      <c r="E24" s="14">
+        <v>2</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="H24" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I24" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
mail to all tutors, mail when tutor is accepted
</commit_message>
<xml_diff>
--- a/01_Planning/ProductBacklog/ProductBacklog.xlsx
+++ b/01_Planning/ProductBacklog/ProductBacklog.xlsx
@@ -316,10 +316,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -655,7 +654,7 @@
   <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -694,659 +693,659 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>1</v>
       </c>
-      <c r="E2" s="6">
-        <v>2</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="I2" s="7" t="s">
+      <c r="E2" s="5">
+        <v>2</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="6">
-        <v>2</v>
-      </c>
-      <c r="E3" s="6">
+      <c r="D3" s="5">
+        <v>2</v>
+      </c>
+      <c r="E3" s="5">
         <v>5</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="I3" s="7" t="s">
+      <c r="F3" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="6">
-        <v>2</v>
-      </c>
-      <c r="E4" s="6">
-        <v>2</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="I4" s="7" t="s">
+      <c r="D4" s="5">
+        <v>2</v>
+      </c>
+      <c r="E4" s="5">
+        <v>2</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="6">
-        <v>2</v>
-      </c>
-      <c r="E5" s="6">
+      <c r="D5" s="5">
+        <v>2</v>
+      </c>
+      <c r="E5" s="5">
         <v>1</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="I5" s="3" t="s">
+      <c r="F5" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="6">
-        <v>2</v>
-      </c>
-      <c r="E6" s="6">
-        <v>2</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="I6" s="7" t="s">
+      <c r="D6" s="5">
+        <v>2</v>
+      </c>
+      <c r="E6" s="5">
+        <v>2</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="6">
-        <v>2</v>
-      </c>
-      <c r="E7" s="6">
+      <c r="D7" s="5">
+        <v>2</v>
+      </c>
+      <c r="E7" s="5">
         <v>1</v>
       </c>
-      <c r="F7" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>38</v>
+      <c r="F7" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="6">
-        <v>2</v>
-      </c>
-      <c r="E8" s="6">
+      <c r="D8" s="5">
+        <v>2</v>
+      </c>
+      <c r="E8" s="5">
         <v>3</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="I8" s="3" t="s">
+      <c r="F8" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>3</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="7">
         <v>3</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="I9" s="7" t="s">
+      <c r="F9" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <v>3</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>5</v>
       </c>
-      <c r="F10" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="I10" s="7" t="s">
+      <c r="F10" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I10" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="5">
         <v>3</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <v>8</v>
       </c>
-      <c r="F11" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="I11" s="7" t="s">
+      <c r="F11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="5">
         <v>3</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="8">
         <v>3</v>
       </c>
-      <c r="F12" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="I12" s="7" t="s">
+      <c r="F12" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I12" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="6">
-        <v>2</v>
-      </c>
-      <c r="E13" s="9">
+      <c r="D13" s="5">
+        <v>2</v>
+      </c>
+      <c r="E13" s="8">
         <v>5</v>
       </c>
-      <c r="F13" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="I13" s="7" t="s">
+      <c r="F13" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I13" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="6">
-        <v>2</v>
-      </c>
-      <c r="E14" s="8">
+      <c r="D14" s="5">
+        <v>2</v>
+      </c>
+      <c r="E14" s="7">
         <v>3</v>
       </c>
-      <c r="F14" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="I14" s="7" t="s">
+      <c r="F14" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I14" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="5">
-        <v>2</v>
-      </c>
-      <c r="E15" s="10">
-        <v>2</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="I15" s="11" t="s">
+      <c r="D15" s="4">
+        <v>2</v>
+      </c>
+      <c r="E15" s="9">
+        <v>2</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I15" s="10" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="4">
         <v>3</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="2">
         <v>5</v>
       </c>
-      <c r="F16" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="H16" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="I16" s="11" t="s">
+      <c r="F16" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I16" s="10" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="5">
-        <v>2</v>
-      </c>
-      <c r="E17" s="5">
+      <c r="D17" s="4">
+        <v>2</v>
+      </c>
+      <c r="E17" s="4">
         <v>8</v>
       </c>
-      <c r="F17" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="I17" s="11" t="s">
+      <c r="F17" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I17" s="10" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="5">
-        <v>2</v>
-      </c>
-      <c r="E18" s="3">
+      <c r="D18" s="4">
+        <v>2</v>
+      </c>
+      <c r="E18" s="2">
         <v>5</v>
       </c>
-      <c r="F18" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="I18" s="11" t="s">
+      <c r="F18" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I18" s="10" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="5">
-        <v>2</v>
-      </c>
-      <c r="E19" s="5">
+      <c r="D19" s="4">
+        <v>2</v>
+      </c>
+      <c r="E19" s="4">
         <v>5</v>
       </c>
-      <c r="F19" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="I19" s="11" t="s">
+      <c r="F19" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I19" s="10" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D20" s="5">
-        <v>2</v>
-      </c>
-      <c r="E20" s="5">
+      <c r="D20" s="4">
+        <v>2</v>
+      </c>
+      <c r="E20" s="4">
         <v>1</v>
       </c>
-      <c r="F20" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="I20" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="13"/>
-      <c r="Q20" s="13"/>
+      <c r="F20" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
+      <c r="Q20" s="12"/>
     </row>
     <row r="21" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D21" s="5">
-        <v>2</v>
-      </c>
-      <c r="E21" s="5">
+      <c r="D21" s="4">
+        <v>2</v>
+      </c>
+      <c r="E21" s="4">
         <v>3</v>
       </c>
-      <c r="F21" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="H21" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="I21" s="11" t="s">
+      <c r="F21" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I21" s="10" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="D22" s="14">
+      <c r="D22" s="13">
         <v>1</v>
       </c>
-      <c r="E22" s="14">
+      <c r="E22" s="13">
         <v>5</v>
       </c>
-      <c r="F22" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="G22" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="H22" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="I22" s="15" t="s">
+      <c r="F22" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H22" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I22" s="14" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="D23" s="14">
-        <v>2</v>
-      </c>
-      <c r="E23" s="14">
-        <v>2</v>
-      </c>
-      <c r="F23" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="G23" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="H23" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="I23" s="15" t="s">
+      <c r="D23" s="13">
+        <v>2</v>
+      </c>
+      <c r="E23" s="13">
+        <v>2</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H23" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I23" s="14" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="D24" s="14">
-        <v>2</v>
-      </c>
-      <c r="E24" s="14">
-        <v>2</v>
-      </c>
-      <c r="F24" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="G24" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="H24" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="I24" s="15" t="s">
+      <c r="D24" s="13">
+        <v>2</v>
+      </c>
+      <c r="E24" s="13">
+        <v>2</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H24" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I24" s="14" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>